<commit_message>
added region stats to separate folder
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\meas\Interference-ScottMcNeil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\meas\p3388_interf_meas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761D5DC2-84F4-4D2E-ADDC-AA6746D16A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B842D1-A882-418B-B88E-F934DFEEECB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3255" yWindow="5175" windowWidth="20490" windowHeight="9315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1605" yWindow="4590" windowWidth="33900" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -89,16 +89,19 @@
     <t>Infrared Curing Machine</t>
   </si>
   <si>
-    <t>Noise Interference from Unshielded VFD</t>
-  </si>
-  <si>
-    <t>Gantry Crane with Unshielded VFD</t>
-  </si>
-  <si>
-    <t>Industrial Microwave Dryer First Meas</t>
-  </si>
-  <si>
-    <t>Industrial Microwave Dryer Second Meas</t>
+    <t>Unshielded VFD</t>
+  </si>
+  <si>
+    <t>Crane with Unshielded VFD</t>
+  </si>
+  <si>
+    <t>Microwave Dryer Take 2</t>
+  </si>
+  <si>
+    <t>Microwave Dryer Take 1</t>
+  </si>
+  <si>
+    <t>Hz</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,10 +469,13 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -529,7 +535,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>

</xml_diff>